<commit_message>
Added type to unregistered students.
</commit_message>
<xml_diff>
--- a/public/examples/example-with-data.xlsx
+++ b/public/examples/example-with-data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -28,12 +28,18 @@
     <t xml:space="preserve">Code</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date</t>
   </si>
   <si>
     <t xml:space="preserve">Yad</t>
   </si>
   <si>
+    <t xml:space="preserve">پارالێل</t>
+  </si>
+  <si>
     <t xml:space="preserve">Yad1</t>
   </si>
   <si>
@@ -44,6 +50,9 @@
   </si>
   <si>
     <t xml:space="preserve">Yad4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">بەیانیان</t>
   </si>
   <si>
     <t xml:space="preserve">Yad5</t>
@@ -137,7 +146,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,10 +273,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -282,101 +291,128 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>111</v>
       </c>
-      <c r="C2" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="n">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>113</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="D4" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>114</v>
       </c>
-      <c r="C5" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="0" t="n">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>115</v>
       </c>
-      <c r="C6" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="0" t="n">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="C7" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="0" t="n">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="C8" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="0" t="n">
-        <v>118</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <f aca="true">TODAY()</f>
-        <v>45281</v>
+      <c r="D9" s="2" t="n">
+        <f aca="true">TODAY()</f>
+        <v>45295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>